<commit_message>
updated with right columns and added sean ohair
</commit_message>
<xml_diff>
--- a/data/PGA Stats.xlsx
+++ b/data/PGA Stats.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-29060" yWindow="-3700" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="200" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PGA Stats.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="1149">
   <si>
     <t>TIGER WOODS - 2013 STATS</t>
   </si>
@@ -3232,6 +3232,240 @@
   </si>
   <si>
     <t>Tot. Strks - 1273</t>
+  </si>
+  <si>
+    <t>Sean O'Hair</t>
+  </si>
+  <si>
+    <t>SEAN O'HAIR - 2013 STATS</t>
+  </si>
+  <si>
+    <t>Tot. Dist. - 32,331</t>
+  </si>
+  <si>
+    <t>Fwys Hit - 419</t>
+  </si>
+  <si>
+    <t>Poss. Fwys - 750</t>
+  </si>
+  <si>
+    <t>167th</t>
+  </si>
+  <si>
+    <t>Greens Hit - 601</t>
+  </si>
+  <si>
+    <t>Total Putts Gained - -11.494</t>
+  </si>
+  <si>
+    <t>Measured Rounds - 49</t>
+  </si>
+  <si>
+    <t># Birdies - 159</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 3,900</t>
+  </si>
+  <si>
+    <t>Tot. Adj. - 4.793-</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 2,298</t>
+  </si>
+  <si>
+    <t># of Top 10's -</t>
+  </si>
+  <si>
+    <t>#Bird/Eagl - 165</t>
+  </si>
+  <si>
+    <t>Greens Hit - 27</t>
+  </si>
+  <si>
+    <t># Holes - 55</t>
+  </si>
+  <si>
+    <t>Par3 Birds - 28</t>
+  </si>
+  <si>
+    <t>Par3 holes - 28</t>
+  </si>
+  <si>
+    <t>Par4 Birds - 62</t>
+  </si>
+  <si>
+    <t>Par4 holes - 62</t>
+  </si>
+  <si>
+    <t>Par5 holes - 69</t>
+  </si>
+  <si>
+    <t># Birdies - 152</t>
+  </si>
+  <si>
+    <t>Greens Hit - 600</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 2,956</t>
+  </si>
+  <si>
+    <t>Tot. Rnds. - 41</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 572</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 516</t>
+  </si>
+  <si>
+    <t>SEAN O'HAIR - 2012 STATS</t>
+  </si>
+  <si>
+    <t>Tot. Dist. - 49,980</t>
+  </si>
+  <si>
+    <t>Tot. Drvs. - 168</t>
+  </si>
+  <si>
+    <t>Fwys Hit - 706</t>
+  </si>
+  <si>
+    <t>Poss. Fwys - 1,177</t>
+  </si>
+  <si>
+    <t>Greens Hit - 1,032</t>
+  </si>
+  <si>
+    <t># Holes - 1,512</t>
+  </si>
+  <si>
+    <t># Eagles - 9</t>
+  </si>
+  <si>
+    <t># Birdies - 311</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 5,937</t>
+  </si>
+  <si>
+    <t>Tot. Adj. - 5.358-</t>
+  </si>
+  <si>
+    <t># Bunkers - 138</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 1,625</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 6,555</t>
+  </si>
+  <si>
+    <t>BonusMoney - 75,000</t>
+  </si>
+  <si>
+    <t>84th</t>
+  </si>
+  <si>
+    <t>#Holes - 1,512</t>
+  </si>
+  <si>
+    <t>Par3 Birds - 52</t>
+  </si>
+  <si>
+    <t>Par3 holes - 52</t>
+  </si>
+  <si>
+    <t>Par4 Birds - 141</t>
+  </si>
+  <si>
+    <t>Par4 holes - 139</t>
+  </si>
+  <si>
+    <t>Par5 holes - 120</t>
+  </si>
+  <si>
+    <t># Birdies - 303</t>
+  </si>
+  <si>
+    <t>Greens Hit - 1,029</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 3,317</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 1,330</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 1,359</t>
+  </si>
+  <si>
+    <t>SEAN O'HAIR - 2011 STATS</t>
+  </si>
+  <si>
+    <t>Tot. Dist. - 41,241</t>
+  </si>
+  <si>
+    <t>Tot. Drvs. - 140</t>
+  </si>
+  <si>
+    <t>Fwys Hit - 545</t>
+  </si>
+  <si>
+    <t>Poss. Fwys - 977</t>
+  </si>
+  <si>
+    <t>Greens Hit - 796</t>
+  </si>
+  <si>
+    <t># Holes - 1,260</t>
+  </si>
+  <si>
+    <t># Birdies - 223</t>
+  </si>
+  <si>
+    <t>Tot. Rnds. - 70</t>
+  </si>
+  <si>
+    <t>88th</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 4,990</t>
+  </si>
+  <si>
+    <t>Tot. Adj. - 33.314-</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 1,182</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 4,159</t>
+  </si>
+  <si>
+    <t>BonusMoney - 110,000</t>
+  </si>
+  <si>
+    <t>#Bird/Eagl - 229</t>
+  </si>
+  <si>
+    <t>#Holes - 1,260</t>
+  </si>
+  <si>
+    <t>Par4 holes - 114</t>
+  </si>
+  <si>
+    <t>Par5 holes - 73</t>
+  </si>
+  <si>
+    <t># Birdies - 215</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 3,365</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 838</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 856</t>
   </si>
 </sst>
 </file>
@@ -3290,8 +3524,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3326,7 +3562,7 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3340,6 +3576,7 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3353,6 +3590,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3682,11 +3920,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD128"/>
+  <dimension ref="A1:AG128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="AG4" sqref="AG4:AG128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3695,7 +3933,7 @@
     <col min="4" max="30" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:33">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -3786,8 +4024,17 @@
       <c r="AD1" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="AE1" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AF1" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>1071</v>
+      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:33">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -3878,8 +4125,17 @@
       <c r="AD2" s="4">
         <v>2011</v>
       </c>
+      <c r="AE2" s="4">
+        <v>2013</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>2012</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>2011</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:33">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3970,8 +4226,17 @@
       <c r="AD4" t="s">
         <v>351</v>
       </c>
+      <c r="AE4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>1099</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>1126</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:33">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4062,8 +4327,17 @@
       <c r="AD5" t="s">
         <v>1</v>
       </c>
+      <c r="AE5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:33">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -4154,8 +4428,17 @@
       <c r="AD6" t="s">
         <v>2</v>
       </c>
+      <c r="AE6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:33">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4246,8 +4529,17 @@
       <c r="AD7" t="s">
         <v>3</v>
       </c>
+      <c r="AE7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:33">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4338,8 +4630,17 @@
       <c r="AD8" t="s">
         <v>4</v>
       </c>
+      <c r="AE8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:33">
       <c r="A9">
         <v>294.5</v>
       </c>
@@ -4430,8 +4731,17 @@
       <c r="AD9">
         <v>272</v>
       </c>
+      <c r="AE9">
+        <v>299.39999999999998</v>
+      </c>
+      <c r="AF9">
+        <v>297.5</v>
+      </c>
+      <c r="AG9">
+        <v>294.60000000000002</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:33">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4522,8 +4832,17 @@
       <c r="AD10" t="s">
         <v>119</v>
       </c>
+      <c r="AE10" t="s">
+        <v>428</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>400</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:33">
       <c r="A11" t="s">
         <v>859</v>
       </c>
@@ -4614,8 +4933,17 @@
       <c r="AD11" t="s">
         <v>888</v>
       </c>
+      <c r="AE11" t="s">
+        <v>1073</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>1100</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>1127</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:33">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -4706,8 +5034,17 @@
       <c r="AD12" t="s">
         <v>352</v>
       </c>
+      <c r="AE12" t="s">
+        <v>465</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>1101</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>1128</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:33">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4798,8 +5135,17 @@
       <c r="AD13" t="s">
         <v>7</v>
       </c>
+      <c r="AE13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:33">
       <c r="A14" s="1">
         <v>0.62280000000000002</v>
       </c>
@@ -4890,8 +5236,17 @@
       <c r="AD14" s="1">
         <v>0.74050000000000005</v>
       </c>
+      <c r="AE14" s="1">
+        <v>0.55869999999999997</v>
+      </c>
+      <c r="AF14" s="1">
+        <v>0.5998</v>
+      </c>
+      <c r="AG14" s="1">
+        <v>0.55779999999999996</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:33">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -4982,8 +5337,17 @@
       <c r="AD15" t="s">
         <v>44</v>
       </c>
+      <c r="AE15" t="s">
+        <v>209</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>313</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>440</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:33">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -5074,8 +5438,17 @@
       <c r="AD16" t="s">
         <v>353</v>
       </c>
+      <c r="AE16" t="s">
+        <v>1074</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>1102</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>1129</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:33">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -5166,8 +5539,17 @@
       <c r="AD17" t="s">
         <v>354</v>
       </c>
+      <c r="AE17" t="s">
+        <v>1075</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>1103</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>1130</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:33">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -5258,8 +5640,17 @@
       <c r="AD18" t="s">
         <v>11</v>
       </c>
+      <c r="AE18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:33">
       <c r="A19" s="1">
         <v>0.67190000000000005</v>
       </c>
@@ -5350,8 +5741,17 @@
       <c r="AD19" s="1">
         <v>0.75760000000000005</v>
       </c>
+      <c r="AE19" s="1">
+        <v>0.61829999999999996</v>
+      </c>
+      <c r="AF19" s="1">
+        <v>0.6825</v>
+      </c>
+      <c r="AG19" s="1">
+        <v>0.63170000000000004</v>
+      </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:33">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -5442,8 +5842,17 @@
       <c r="AD20" t="s">
         <v>20</v>
       </c>
+      <c r="AE20" t="s">
+        <v>1076</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>436</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>610</v>
+      </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:33">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -5534,8 +5943,17 @@
       <c r="AD21" t="s">
         <v>355</v>
       </c>
+      <c r="AE21" t="s">
+        <v>1077</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>1104</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>1131</v>
+      </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:33">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -5626,8 +6044,17 @@
       <c r="AD22" t="s">
         <v>356</v>
       </c>
+      <c r="AE22" t="s">
+        <v>470</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>1105</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>1132</v>
+      </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:33">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -5718,8 +6145,17 @@
       <c r="AD23" t="s">
         <v>15</v>
       </c>
+      <c r="AE23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:33">
       <c r="A24">
         <v>0.83299999999999996</v>
       </c>
@@ -5810,8 +6246,17 @@
       <c r="AD24">
         <v>0.39600000000000002</v>
       </c>
+      <c r="AE24">
+        <v>-0.23499999999999999</v>
+      </c>
+      <c r="AF24">
+        <v>-0.30199999999999999</v>
+      </c>
+      <c r="AG24">
+        <v>-0.22</v>
+      </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:33">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -5902,8 +6347,17 @@
       <c r="AD25" t="s">
         <v>222</v>
       </c>
+      <c r="AE25" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>455</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:33">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -5994,8 +6448,17 @@
       <c r="AD26" t="s">
         <v>41</v>
       </c>
+      <c r="AE26" t="s">
+        <v>1078</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:33">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -6086,8 +6549,17 @@
       <c r="AD27" t="s">
         <v>41</v>
       </c>
+      <c r="AE27" t="s">
+        <v>1079</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:33">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -6178,8 +6650,17 @@
       <c r="AD28" t="s">
         <v>22</v>
       </c>
+      <c r="AE28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:33">
       <c r="A29">
         <v>82.3</v>
       </c>
@@ -6270,8 +6751,17 @@
       <c r="AD29">
         <v>4.09</v>
       </c>
+      <c r="AE29">
+        <v>162</v>
+      </c>
+      <c r="AF29">
+        <v>168</v>
+      </c>
+      <c r="AG29">
+        <v>210</v>
+      </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:33">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -6362,8 +6852,17 @@
       <c r="AD30" t="s">
         <v>357</v>
       </c>
+      <c r="AE30" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>835</v>
+      </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:33">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -6454,8 +6953,17 @@
       <c r="AD31" t="s">
         <v>358</v>
       </c>
+      <c r="AE31" t="s">
+        <v>470</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>1105</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>1132</v>
+      </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:33">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -6546,8 +7054,17 @@
       <c r="AD32" t="s">
         <v>348</v>
       </c>
+      <c r="AE32" t="s">
+        <v>323</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>1106</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>323</v>
+      </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:33">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -6638,8 +7155,17 @@
       <c r="AD33" t="s">
         <v>26</v>
       </c>
+      <c r="AE33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:33">
       <c r="A34">
         <v>4.1900000000000004</v>
       </c>
@@ -6730,8 +7256,17 @@
       <c r="AD34">
         <v>70.849999999999994</v>
       </c>
+      <c r="AE34">
+        <v>2.94</v>
+      </c>
+      <c r="AF34">
+        <v>3.7</v>
+      </c>
+      <c r="AG34">
+        <v>3.19</v>
+      </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:33">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -6822,8 +7357,17 @@
       <c r="AD35" t="s">
         <v>262</v>
       </c>
+      <c r="AE35" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>455</v>
+      </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:33">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -6914,8 +7458,17 @@
       <c r="AD36" t="s">
         <v>359</v>
       </c>
+      <c r="AE36" t="s">
+        <v>1080</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>1107</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>1133</v>
+      </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:33">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -7006,8 +7559,17 @@
       <c r="AD37" t="s">
         <v>360</v>
       </c>
+      <c r="AE37" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>423</v>
+      </c>
+      <c r="AG37" t="s">
+        <v>1134</v>
+      </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:33">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -7098,8 +7660,17 @@
       <c r="AD38" t="s">
         <v>28</v>
       </c>
+      <c r="AE38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG38" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:33">
       <c r="A39">
         <v>69.081999999999994</v>
       </c>
@@ -7190,8 +7761,17 @@
       <c r="AD39" s="1">
         <v>0.58330000000000004</v>
       </c>
+      <c r="AE39">
+        <v>72.132999999999996</v>
+      </c>
+      <c r="AF39">
+        <v>70.614999999999995</v>
+      </c>
+      <c r="AG39">
+        <v>70.81</v>
+      </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:33">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -7282,8 +7862,17 @@
       <c r="AD40" t="s">
         <v>361</v>
       </c>
+      <c r="AE40" t="s">
+        <v>334</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>1135</v>
+      </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:33">
       <c r="A41" t="s">
         <v>924</v>
       </c>
@@ -7374,8 +7963,17 @@
       <c r="AD41" t="s">
         <v>362</v>
       </c>
+      <c r="AE41" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>1136</v>
+      </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:33">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -7466,8 +8064,17 @@
       <c r="AD42" t="s">
         <v>363</v>
       </c>
+      <c r="AE42" t="s">
+        <v>1082</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>1109</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>1137</v>
+      </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:33">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -7558,8 +8165,17 @@
       <c r="AD43" t="s">
         <v>32</v>
       </c>
+      <c r="AE43" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>28</v>
+      </c>
+      <c r="AG43" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:33">
       <c r="A44" s="1">
         <v>0.59260000000000002</v>
       </c>
@@ -7650,8 +8266,17 @@
       <c r="AD44" s="2">
         <v>1998</v>
       </c>
+      <c r="AE44" s="1">
+        <v>0.4824</v>
+      </c>
+      <c r="AF44" s="1">
+        <v>0.44929999999999998</v>
+      </c>
+      <c r="AG44" s="1">
+        <v>0.48</v>
+      </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:33">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -7742,8 +8367,17 @@
       <c r="AD45" t="s">
         <v>119</v>
       </c>
+      <c r="AE45" t="s">
+        <v>468</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>397</v>
+      </c>
+      <c r="AG45" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:33">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -7834,8 +8468,17 @@
       <c r="AD46" t="s">
         <v>34</v>
       </c>
+      <c r="AE46" t="s">
+        <v>608</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>449</v>
+      </c>
+      <c r="AG46" t="s">
+        <v>791</v>
+      </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:33">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -7926,8 +8569,17 @@
       <c r="AD47" t="s">
         <v>98</v>
       </c>
+      <c r="AE47" t="s">
+        <v>636</v>
+      </c>
+      <c r="AF47" t="s">
+        <v>1110</v>
+      </c>
+      <c r="AG47" t="s">
+        <v>96</v>
+      </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:33">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -8018,8 +8670,17 @@
       <c r="AD48">
         <v>299</v>
       </c>
+      <c r="AE48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG48" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:33">
       <c r="A49">
         <v>103</v>
       </c>
@@ -8110,8 +8771,17 @@
       <c r="AD49" t="s">
         <v>364</v>
       </c>
+      <c r="AE49">
+        <v>181</v>
+      </c>
+      <c r="AF49">
+        <v>149</v>
+      </c>
+      <c r="AG49">
+        <v>227</v>
+      </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:33">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -8202,8 +8872,17 @@
       <c r="AD50" t="s">
         <v>952</v>
       </c>
+      <c r="AE50" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>826</v>
+      </c>
+      <c r="AG50" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:33">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -8294,8 +8973,17 @@
       <c r="AD51" t="s">
         <v>41</v>
       </c>
+      <c r="AE51" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:33">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -8386,8 +9074,17 @@
       <c r="AD52" t="s">
         <v>99</v>
       </c>
+      <c r="AE52" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG52" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:33">
       <c r="A53">
         <v>175</v>
       </c>
@@ -8478,8 +9175,17 @@
       <c r="AD53">
         <v>299</v>
       </c>
+      <c r="AE53" s="2">
+        <v>1027</v>
+      </c>
+      <c r="AF53">
+        <v>559</v>
+      </c>
+      <c r="AG53">
+        <v>973</v>
+      </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:33">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -8570,8 +9276,17 @@
       <c r="AD54" t="s">
         <v>364</v>
       </c>
+      <c r="AE54" t="s">
+        <v>440</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>826</v>
+      </c>
+      <c r="AG54" t="s">
+        <v>553</v>
+      </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:33">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -8662,8 +9377,17 @@
       <c r="AD55" t="s">
         <v>954</v>
       </c>
+      <c r="AE55" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF55" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG55" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:33">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -8754,8 +9478,17 @@
       <c r="AD56" t="s">
         <v>955</v>
       </c>
+      <c r="AE56" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF56" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG56" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:33">
       <c r="A57" s="2">
         <v>2380</v>
       </c>
@@ -8846,8 +9579,17 @@
       <c r="AD57" t="s">
         <v>40</v>
       </c>
+      <c r="AE57">
+        <v>183</v>
+      </c>
+      <c r="AF57">
+        <v>644</v>
+      </c>
+      <c r="AG57">
+        <v>724</v>
+      </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:33">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -8938,8 +9680,17 @@
       <c r="AD58" s="3">
         <v>571000</v>
       </c>
+      <c r="AE58" t="s">
+        <v>229</v>
+      </c>
+      <c r="AF58" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG58" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:33">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -9030,8 +9781,17 @@
       <c r="AD59" t="s">
         <v>365</v>
       </c>
+      <c r="AE59" t="s">
+        <v>1083</v>
+      </c>
+      <c r="AF59" t="s">
+        <v>1111</v>
+      </c>
+      <c r="AG59" t="s">
+        <v>1138</v>
+      </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:33">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -9122,8 +9882,17 @@
       <c r="AD60" t="s">
         <v>41</v>
       </c>
+      <c r="AE60" t="s">
+        <v>1084</v>
+      </c>
+      <c r="AF60" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG60" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:33">
       <c r="A61" t="s">
         <v>40</v>
       </c>
@@ -9214,8 +9983,17 @@
       <c r="AD61" t="s">
         <v>41</v>
       </c>
+      <c r="AE61" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF61" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG61" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:33">
       <c r="A62" s="3">
         <v>5909742</v>
       </c>
@@ -9306,8 +10084,17 @@
       <c r="AD62" t="s">
         <v>43</v>
       </c>
+      <c r="AE62" s="3">
+        <v>268614</v>
+      </c>
+      <c r="AF62">
+        <v>744</v>
+      </c>
+      <c r="AG62" s="2">
+        <v>1102</v>
+      </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:33">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -9398,8 +10185,17 @@
       <c r="AD63" s="1">
         <v>0.2273</v>
       </c>
+      <c r="AE63" t="s">
+        <v>455</v>
+      </c>
+      <c r="AF63" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG63" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:33">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -9490,8 +10286,17 @@
       <c r="AD64" t="s">
         <v>225</v>
       </c>
+      <c r="AE64" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF64" t="s">
+        <v>1112</v>
+      </c>
+      <c r="AG64" t="s">
+        <v>1139</v>
+      </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:33">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -9582,8 +10387,17 @@
       <c r="AD65" t="s">
         <v>366</v>
       </c>
+      <c r="AE65" t="s">
+        <v>189</v>
+      </c>
+      <c r="AF65" t="s">
+        <v>1113</v>
+      </c>
+      <c r="AG65" t="s">
+        <v>1140</v>
+      </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:33">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -9674,8 +10488,17 @@
       <c r="AD66" t="s">
         <v>367</v>
       </c>
+      <c r="AE66" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF66" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG66" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:33">
       <c r="A67" s="1">
         <v>0.24479999999999999</v>
       </c>
@@ -9766,8 +10589,17 @@
       <c r="AD67" t="s">
         <v>47</v>
       </c>
+      <c r="AE67" s="1">
+        <v>0.16980000000000001</v>
+      </c>
+      <c r="AF67" s="3">
+        <v>1160981</v>
+      </c>
+      <c r="AG67" s="3">
+        <v>1483948</v>
+      </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:33">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -9858,8 +10690,17 @@
       <c r="AD68" s="1">
         <v>0.5</v>
       </c>
+      <c r="AE68" t="s">
+        <v>435</v>
+      </c>
+      <c r="AF68" t="s">
+        <v>1114</v>
+      </c>
+      <c r="AG68" t="s">
+        <v>374</v>
+      </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:33">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -9950,8 +10791,17 @@
       <c r="AD69" t="s">
         <v>296</v>
       </c>
+      <c r="AE69" t="s">
+        <v>1085</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:33">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -10042,8 +10892,17 @@
       <c r="AD70" t="s">
         <v>41</v>
       </c>
+      <c r="AE70" t="s">
+        <v>481</v>
+      </c>
+      <c r="AF70" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG70" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:33">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -10134,8 +10993,17 @@
       <c r="AD71" t="s">
         <v>41</v>
       </c>
+      <c r="AE71" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF71" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG71" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:33">
       <c r="A72" s="1">
         <v>0.46200000000000002</v>
       </c>
@@ -10226,8 +11094,17 @@
       <c r="AD72" t="s">
         <v>51</v>
       </c>
+      <c r="AE72" s="1">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="AF72" s="1">
+        <v>0.21160000000000001</v>
+      </c>
+      <c r="AG72" s="1">
+        <v>0.1817</v>
+      </c>
     </row>
-    <row r="73" spans="1:30">
+    <row r="73" spans="1:33">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -10318,8 +11195,17 @@
       <c r="AD73" t="s">
         <v>52</v>
       </c>
+      <c r="AE73" t="s">
+        <v>254</v>
+      </c>
+      <c r="AF73" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG73" t="s">
+        <v>440</v>
+      </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:33">
       <c r="A74" t="s">
         <v>49</v>
       </c>
@@ -10410,8 +11296,17 @@
       <c r="AD74" t="s">
         <v>2</v>
       </c>
+      <c r="AE74" t="s">
+        <v>1086</v>
+      </c>
+      <c r="AF74" t="s">
+        <v>850</v>
+      </c>
+      <c r="AG74" t="s">
+        <v>1141</v>
+      </c>
     </row>
-    <row r="75" spans="1:30">
+    <row r="75" spans="1:33">
       <c r="A75" t="s">
         <v>50</v>
       </c>
@@ -10502,8 +11397,17 @@
       <c r="AD75" t="s">
         <v>3</v>
       </c>
+      <c r="AE75" t="s">
+        <v>1087</v>
+      </c>
+      <c r="AF75" t="s">
+        <v>1115</v>
+      </c>
+      <c r="AG75" t="s">
+        <v>1142</v>
+      </c>
     </row>
-    <row r="76" spans="1:30">
+    <row r="76" spans="1:33">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -10594,8 +11498,17 @@
       <c r="AD76" t="s">
         <v>53</v>
       </c>
+      <c r="AE76" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF76" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG76" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:33">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -10686,8 +11599,17 @@
       <c r="AD77" s="1">
         <v>0.15</v>
       </c>
+      <c r="AE77" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF77" s="1">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="AG77" s="1">
+        <v>0.40699999999999997</v>
+      </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:33">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -10778,8 +11700,17 @@
       <c r="AD78" t="s">
         <v>193</v>
       </c>
+      <c r="AE78" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF78" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG78" t="s">
+        <v>287</v>
+      </c>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:33">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -10870,8 +11801,17 @@
       <c r="AD79" t="s">
         <v>368</v>
       </c>
+      <c r="AE79" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF79" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG79" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:33">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -10962,8 +11902,17 @@
       <c r="AD80" t="s">
         <v>369</v>
       </c>
+      <c r="AE80" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF80" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG80" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:33">
       <c r="A81" s="1">
         <v>0.1484</v>
       </c>
@@ -11054,8 +12003,17 @@
       <c r="AD81" t="s">
         <v>57</v>
       </c>
+      <c r="AE81" s="1">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="AF81" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG81" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:33">
       <c r="A82" t="s">
         <v>54</v>
       </c>
@@ -11146,8 +12104,17 @@
       <c r="AD82" s="1">
         <v>0.1721</v>
       </c>
+      <c r="AE82" t="s">
+        <v>518</v>
+      </c>
+      <c r="AF82" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG82" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:33">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -11238,8 +12205,17 @@
       <c r="AD83" t="s">
         <v>104</v>
       </c>
+      <c r="AE83" t="s">
+        <v>1088</v>
+      </c>
+      <c r="AF83" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG83" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:33">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -11330,8 +12306,17 @@
       <c r="AD84" t="s">
         <v>370</v>
       </c>
+      <c r="AE84" t="s">
+        <v>1089</v>
+      </c>
+      <c r="AF84" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG84" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:33">
       <c r="A85" t="s">
         <v>57</v>
       </c>
@@ -11422,8 +12407,17 @@
       <c r="AD85" t="s">
         <v>371</v>
       </c>
+      <c r="AE85" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF85" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG85" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:33">
       <c r="A86" s="1">
         <v>0.17560000000000001</v>
       </c>
@@ -11514,8 +12508,17 @@
       <c r="AD86" t="s">
         <v>61</v>
       </c>
+      <c r="AE86" s="1">
+        <v>0.1082</v>
+      </c>
+      <c r="AF86" s="1">
+        <v>0.1552</v>
+      </c>
+      <c r="AG86" s="1">
+        <v>0.12720000000000001</v>
+      </c>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:33">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -11606,8 +12609,17 @@
       <c r="AD87" s="1">
         <v>0.5</v>
       </c>
+      <c r="AE87" t="s">
+        <v>573</v>
+      </c>
+      <c r="AF87" t="s">
+        <v>413</v>
+      </c>
+      <c r="AG87" t="s">
+        <v>313</v>
+      </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:33">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -11698,8 +12710,17 @@
       <c r="AD88" t="s">
         <v>107</v>
       </c>
+      <c r="AE88" t="s">
+        <v>1090</v>
+      </c>
+      <c r="AF88" t="s">
+        <v>1116</v>
+      </c>
+      <c r="AG88" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:33">
       <c r="A89" t="s">
         <v>60</v>
       </c>
@@ -11790,8 +12811,17 @@
       <c r="AD89" t="s">
         <v>372</v>
       </c>
+      <c r="AE89" t="s">
+        <v>1091</v>
+      </c>
+      <c r="AF89" t="s">
+        <v>1117</v>
+      </c>
+      <c r="AG89" t="s">
+        <v>267</v>
+      </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:33">
       <c r="A90" t="s">
         <v>61</v>
       </c>
@@ -11882,8 +12912,17 @@
       <c r="AD90" t="s">
         <v>373</v>
       </c>
+      <c r="AE90" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF90" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG90" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:33">
       <c r="A91" s="1">
         <v>0.5625</v>
       </c>
@@ -11974,8 +13013,17 @@
       <c r="AD91" t="s">
         <v>65</v>
       </c>
+      <c r="AE91" s="1">
+        <v>0.42370000000000002</v>
+      </c>
+      <c r="AF91" s="1">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="AG91" s="1">
+        <v>0.1454</v>
+      </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:33">
       <c r="A92" t="s">
         <v>62</v>
       </c>
@@ -12066,8 +13114,17 @@
       <c r="AD92" s="1">
         <v>0.3</v>
       </c>
+      <c r="AE92" t="s">
+        <v>473</v>
+      </c>
+      <c r="AF92" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG92" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:33">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -12158,8 +13215,17 @@
       <c r="AD93" t="s">
         <v>374</v>
       </c>
+      <c r="AE93" t="s">
+        <v>616</v>
+      </c>
+      <c r="AF93" t="s">
+        <v>1118</v>
+      </c>
+      <c r="AG93" t="s">
+        <v>614</v>
+      </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:33">
       <c r="A94" t="s">
         <v>64</v>
       </c>
@@ -12250,8 +13316,17 @@
       <c r="AD94" t="s">
         <v>358</v>
       </c>
+      <c r="AE94" t="s">
+        <v>1092</v>
+      </c>
+      <c r="AF94" t="s">
+        <v>1119</v>
+      </c>
+      <c r="AG94" t="s">
+        <v>1143</v>
+      </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:33">
       <c r="A95" t="s">
         <v>65</v>
       </c>
@@ -12342,8 +13417,17 @@
       <c r="AD95" t="s">
         <v>355</v>
       </c>
+      <c r="AE95" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF95" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG95" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:33">
       <c r="A96" s="1">
         <v>0.3523</v>
       </c>
@@ -12434,8 +13518,17 @@
       <c r="AD96" t="s">
         <v>51</v>
       </c>
+      <c r="AE96" s="1">
+        <v>0.25330000000000003</v>
+      </c>
+      <c r="AF96" s="1">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="AG96" s="1">
+        <v>0.4093</v>
+      </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:33">
       <c r="A97" t="s">
         <v>44</v>
       </c>
@@ -12526,8 +13619,17 @@
       <c r="AD97" t="s">
         <v>68</v>
       </c>
+      <c r="AE97" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF97" t="s">
+        <v>361</v>
+      </c>
+      <c r="AG97" t="s">
+        <v>618</v>
+      </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:33">
       <c r="A98" t="s">
         <v>66</v>
       </c>
@@ -12618,8 +13720,17 @@
       <c r="AD98" t="s">
         <v>2</v>
       </c>
+      <c r="AE98" t="s">
+        <v>1093</v>
+      </c>
+      <c r="AF98" t="s">
+        <v>666</v>
+      </c>
+      <c r="AG98" t="s">
+        <v>822</v>
+      </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:33">
       <c r="A99" t="s">
         <v>67</v>
       </c>
@@ -12710,8 +13821,17 @@
       <c r="AD99" t="s">
         <v>3</v>
       </c>
+      <c r="AE99" t="s">
+        <v>1094</v>
+      </c>
+      <c r="AF99" t="s">
+        <v>1120</v>
+      </c>
+      <c r="AG99" t="s">
+        <v>1144</v>
+      </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:33">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -12802,8 +13922,17 @@
       <c r="AD100" t="s">
         <v>69</v>
       </c>
+      <c r="AE100" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF100" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG100" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:33">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -12894,8 +14023,17 @@
       <c r="AD101">
         <v>69.73</v>
       </c>
+      <c r="AE101" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF101" s="1">
+        <v>0.29449999999999998</v>
+      </c>
+      <c r="AG101" s="1">
+        <v>0.27010000000000001</v>
+      </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:33">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -12986,8 +14124,17 @@
       <c r="AD102" t="s">
         <v>357</v>
       </c>
+      <c r="AE102" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF102" t="s">
+        <v>288</v>
+      </c>
+      <c r="AG102" t="s">
+        <v>697</v>
+      </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:33">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -13078,8 +14225,17 @@
       <c r="AD103" t="s">
         <v>359</v>
       </c>
+      <c r="AE103" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF103" t="s">
+        <v>1121</v>
+      </c>
+      <c r="AG103" t="s">
+        <v>1145</v>
+      </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:33">
       <c r="A104" t="s">
         <v>69</v>
       </c>
@@ -13170,8 +14326,17 @@
       <c r="AD104" t="s">
         <v>348</v>
       </c>
+      <c r="AE104" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF104" t="s">
+        <v>1122</v>
+      </c>
+      <c r="AG104" t="s">
+        <v>1131</v>
+      </c>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:33">
       <c r="A105">
         <v>70.28</v>
       </c>
@@ -13259,8 +14424,17 @@
       <c r="AD105" t="s">
         <v>71</v>
       </c>
+      <c r="AE105">
+        <v>72.22</v>
+      </c>
+      <c r="AF105" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG105" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:33">
       <c r="A106" t="s">
         <v>70</v>
       </c>
@@ -13348,8 +14522,17 @@
       <c r="AD106">
         <v>70.86</v>
       </c>
+      <c r="AE106" t="s">
+        <v>316</v>
+      </c>
+      <c r="AF106" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG106" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:33">
       <c r="A107" t="s">
         <v>924</v>
       </c>
@@ -13437,8 +14620,17 @@
       <c r="AD107" t="s">
         <v>375</v>
       </c>
+      <c r="AE107" t="s">
+        <v>1081</v>
+      </c>
+      <c r="AF107" t="s">
+        <v>2</v>
+      </c>
+      <c r="AG107" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:33">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -13526,8 +14718,17 @@
       <c r="AD108" t="s">
         <v>376</v>
       </c>
+      <c r="AE108" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF108" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG108" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:33">
       <c r="A109" t="s">
         <v>71</v>
       </c>
@@ -13615,8 +14816,17 @@
       <c r="AD109" t="s">
         <v>377</v>
       </c>
+      <c r="AE109" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF109" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG109" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:33">
       <c r="A110">
         <v>69.25</v>
       </c>
@@ -13704,8 +14914,17 @@
       <c r="AD110" t="s">
         <v>73</v>
       </c>
+      <c r="AE110">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="AF110">
+        <v>70.680000000000007</v>
+      </c>
+      <c r="AG110">
+        <v>71.290000000000006</v>
+      </c>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:33">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -13793,8 +15012,17 @@
       <c r="AD111">
         <v>69.5</v>
       </c>
+      <c r="AE111" t="s">
+        <v>435</v>
+      </c>
+      <c r="AF111" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG111" t="s">
+        <v>443</v>
+      </c>
     </row>
-    <row r="112" spans="1:30">
+    <row r="112" spans="1:33">
       <c r="A112" t="s">
         <v>1020</v>
       </c>
@@ -13882,8 +15110,17 @@
       <c r="AD112" t="s">
         <v>346</v>
       </c>
+      <c r="AE112" t="s">
+        <v>1095</v>
+      </c>
+      <c r="AF112" t="s">
+        <v>1108</v>
+      </c>
+      <c r="AG112" t="s">
+        <v>1136</v>
+      </c>
     </row>
-    <row r="113" spans="1:30">
+    <row r="113" spans="1:33">
       <c r="A113" t="s">
         <v>72</v>
       </c>
@@ -13971,8 +15208,17 @@
       <c r="AD113" t="s">
         <v>378</v>
       </c>
+      <c r="AE113" t="s">
+        <v>1096</v>
+      </c>
+      <c r="AF113" t="s">
+        <v>423</v>
+      </c>
+      <c r="AG113" t="s">
+        <v>1134</v>
+      </c>
     </row>
-    <row r="114" spans="1:30">
+    <row r="114" spans="1:33">
       <c r="A114" t="s">
         <v>73</v>
       </c>
@@ -14060,8 +15306,17 @@
       <c r="AD114" t="s">
         <v>379</v>
       </c>
+      <c r="AE114" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF114" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG114" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="115" spans="1:30">
+    <row r="115" spans="1:33">
       <c r="A115">
         <v>71</v>
       </c>
@@ -14146,8 +15401,17 @@
       <c r="AD115" t="s">
         <v>77</v>
       </c>
+      <c r="AE115">
+        <v>71.5</v>
+      </c>
+      <c r="AF115">
+        <v>70.569999999999993</v>
+      </c>
+      <c r="AG115">
+        <v>71.599999999999994</v>
+      </c>
     </row>
-    <row r="116" spans="1:30">
+    <row r="116" spans="1:33">
       <c r="A116" t="s">
         <v>74</v>
       </c>
@@ -14232,8 +15496,17 @@
       <c r="AD116">
         <v>66</v>
       </c>
+      <c r="AE116" t="s">
+        <v>825</v>
+      </c>
+      <c r="AF116" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG116" t="s">
+        <v>408</v>
+      </c>
     </row>
-    <row r="117" spans="1:30">
+    <row r="117" spans="1:33">
       <c r="A117" t="s">
         <v>75</v>
       </c>
@@ -14318,8 +15591,17 @@
       <c r="AD117" t="s">
         <v>20</v>
       </c>
+      <c r="AE117" t="s">
+        <v>1097</v>
+      </c>
+      <c r="AF117" t="s">
+        <v>1123</v>
+      </c>
+      <c r="AG117" t="s">
+        <v>1146</v>
+      </c>
     </row>
-    <row r="118" spans="1:30">
+    <row r="118" spans="1:33">
       <c r="A118" t="s">
         <v>76</v>
       </c>
@@ -14404,8 +15686,17 @@
       <c r="AD118" t="s">
         <v>380</v>
       </c>
+      <c r="AE118" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF118" t="s">
+        <v>437</v>
+      </c>
+      <c r="AG118" t="s">
+        <v>437</v>
+      </c>
     </row>
-    <row r="119" spans="1:30">
+    <row r="119" spans="1:33">
       <c r="A119" t="s">
         <v>77</v>
       </c>
@@ -14490,8 +15781,17 @@
       <c r="AD119" t="s">
         <v>379</v>
       </c>
+      <c r="AE119" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF119" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG119" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="120" spans="1:30">
+    <row r="120" spans="1:33">
       <c r="A120">
         <v>71.63</v>
       </c>
@@ -14573,8 +15873,17 @@
       <c r="AC120">
         <v>69.91</v>
       </c>
+      <c r="AE120">
+        <v>73.709999999999994</v>
+      </c>
+      <c r="AF120">
+        <v>70</v>
+      </c>
+      <c r="AG120">
+        <v>69.83</v>
+      </c>
     </row>
-    <row r="121" spans="1:30">
+    <row r="121" spans="1:33">
       <c r="A121" t="s">
         <v>78</v>
       </c>
@@ -14656,8 +15965,17 @@
       <c r="AC121" t="s">
         <v>346</v>
       </c>
+      <c r="AE121" t="s">
+        <v>119</v>
+      </c>
+      <c r="AF121" t="s">
+        <v>413</v>
+      </c>
+      <c r="AG121" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="122" spans="1:30">
+    <row r="122" spans="1:33">
       <c r="A122" t="s">
         <v>79</v>
       </c>
@@ -14739,8 +16057,17 @@
       <c r="AC122" t="s">
         <v>347</v>
       </c>
+      <c r="AE122" t="s">
+        <v>1098</v>
+      </c>
+      <c r="AF122" t="s">
+        <v>1124</v>
+      </c>
+      <c r="AG122" t="s">
+        <v>1147</v>
+      </c>
     </row>
-    <row r="123" spans="1:30">
+    <row r="123" spans="1:33">
       <c r="A123" t="s">
         <v>76</v>
       </c>
@@ -14822,8 +16149,17 @@
       <c r="AC123" t="s">
         <v>348</v>
       </c>
+      <c r="AE123" t="s">
+        <v>377</v>
+      </c>
+      <c r="AF123" t="s">
+        <v>438</v>
+      </c>
+      <c r="AG123" t="s">
+        <v>495</v>
+      </c>
     </row>
-    <row r="124" spans="1:30">
+    <row r="124" spans="1:33">
       <c r="B124" t="s">
         <v>77</v>
       </c>
@@ -14875,8 +16211,14 @@
       <c r="AC124" t="s">
         <v>77</v>
       </c>
+      <c r="AF124" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG124" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="125" spans="1:30">
+    <row r="125" spans="1:33">
       <c r="B125">
         <v>70.400000000000006</v>
       </c>
@@ -14925,8 +16267,14 @@
       <c r="AC125">
         <v>70.64</v>
       </c>
+      <c r="AF125">
+        <v>71.53</v>
+      </c>
+      <c r="AG125">
+        <v>71.33</v>
+      </c>
     </row>
-    <row r="126" spans="1:30">
+    <row r="126" spans="1:33">
       <c r="B126" t="s">
         <v>114</v>
       </c>
@@ -14975,8 +16323,14 @@
       <c r="AC126" t="s">
         <v>349</v>
       </c>
+      <c r="AF126" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG126" t="s">
+        <v>540</v>
+      </c>
     </row>
-    <row r="127" spans="1:30">
+    <row r="127" spans="1:33">
       <c r="B127" t="s">
         <v>1060</v>
       </c>
@@ -15025,8 +16379,14 @@
       <c r="AC127" t="s">
         <v>350</v>
       </c>
+      <c r="AF127" t="s">
+        <v>1125</v>
+      </c>
+      <c r="AG127" t="s">
+        <v>1148</v>
+      </c>
     </row>
-    <row r="128" spans="1:30">
+    <row r="128" spans="1:33">
       <c r="B128" t="s">
         <v>115</v>
       </c>
@@ -15074,6 +16434,12 @@
       </c>
       <c r="AC128" t="s">
         <v>348</v>
+      </c>
+      <c r="AF128" t="s">
+        <v>438</v>
+      </c>
+      <c r="AG128" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started the Winnings Stats
</commit_message>
<xml_diff>
--- a/data/PGA Stats.xlsx
+++ b/data/PGA Stats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="1149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="1175">
   <si>
     <t>TIGER WOODS - 2013 STATS</t>
   </si>
@@ -3466,6 +3466,84 @@
   </si>
   <si>
     <t>Tot. Strks - 856</t>
+  </si>
+  <si>
+    <t>SEAN O'HAIR - 2010 STATS</t>
+  </si>
+  <si>
+    <t>Tot. Dist. - 47,162</t>
+  </si>
+  <si>
+    <t>Tot. Drvs. - 163</t>
+  </si>
+  <si>
+    <t>Fwys Hit - 739</t>
+  </si>
+  <si>
+    <t>Poss. Fwys - 1,155</t>
+  </si>
+  <si>
+    <t>Greens Hit - 1,007</t>
+  </si>
+  <si>
+    <t># Holes - 1,476</t>
+  </si>
+  <si>
+    <t># Birdies - 270</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 5,805</t>
+  </si>
+  <si>
+    <t>Tot. Adj. - 15.570-</t>
+  </si>
+  <si>
+    <t># Saves - 66</t>
+  </si>
+  <si>
+    <t># Bunkers - 137</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 988</t>
+  </si>
+  <si>
+    <t>Pts.Behind - 3,729</t>
+  </si>
+  <si>
+    <t>BonusMoney - 128,000</t>
+  </si>
+  <si>
+    <t>#Holes - 1,476</t>
+  </si>
+  <si>
+    <t>Par3 holes - 35</t>
+  </si>
+  <si>
+    <t>Par4 Birds - 137</t>
+  </si>
+  <si>
+    <t>Par4 holes - 136</t>
+  </si>
+  <si>
+    <t>Par5 holes - 99</t>
+  </si>
+  <si>
+    <t># Birdies - 269</t>
+  </si>
+  <si>
+    <t>Greens Hit - 1,005</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 3,464</t>
+  </si>
+  <si>
+    <t>Tot. Rnds. - 49</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 1,273</t>
+  </si>
+  <si>
+    <t>Tot. Strks - 1,137</t>
   </si>
 </sst>
 </file>
@@ -3524,8 +3602,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3562,7 +3642,7 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3577,6 +3657,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3591,6 +3672,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3920,20 +4002,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG128"/>
+  <dimension ref="A1:AH128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG4" sqref="AG4:AG128"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AF109" sqref="AF109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="4" max="30" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="30" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -4033,8 +4116,11 @@
       <c r="AG1" s="4" t="s">
         <v>1071</v>
       </c>
+      <c r="AH1" s="4" t="s">
+        <v>1071</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:34">
       <c r="A2">
         <v>2013</v>
       </c>
@@ -4134,8 +4220,11 @@
       <c r="AG2" s="4">
         <v>2011</v>
       </c>
+      <c r="AH2" s="4">
+        <v>2010</v>
+      </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:34">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -4235,8 +4324,11 @@
       <c r="AG4" t="s">
         <v>1126</v>
       </c>
+      <c r="AH4" t="s">
+        <v>1149</v>
+      </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -4336,8 +4428,11 @@
       <c r="AG5" t="s">
         <v>1</v>
       </c>
+      <c r="AH5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:34">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -4437,8 +4532,11 @@
       <c r="AG6" t="s">
         <v>2</v>
       </c>
+      <c r="AH6" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:34">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -4538,8 +4636,11 @@
       <c r="AG7" t="s">
         <v>3</v>
       </c>
+      <c r="AH7" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:34">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -4639,8 +4740,11 @@
       <c r="AG8" t="s">
         <v>4</v>
       </c>
+      <c r="AH8" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:34">
       <c r="A9">
         <v>294.5</v>
       </c>
@@ -4740,8 +4844,11 @@
       <c r="AG9">
         <v>294.60000000000002</v>
       </c>
+      <c r="AH9">
+        <v>289.3</v>
+      </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:34">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -4841,8 +4948,11 @@
       <c r="AG10" t="s">
         <v>240</v>
       </c>
+      <c r="AH10" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:34">
       <c r="A11" t="s">
         <v>859</v>
       </c>
@@ -4942,8 +5052,11 @@
       <c r="AG11" t="s">
         <v>1127</v>
       </c>
+      <c r="AH11" t="s">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:34">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -5043,8 +5156,11 @@
       <c r="AG12" t="s">
         <v>1128</v>
       </c>
+      <c r="AH12" t="s">
+        <v>1151</v>
+      </c>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:34">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -5144,8 +5260,11 @@
       <c r="AG13" t="s">
         <v>7</v>
       </c>
+      <c r="AH13" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:34">
       <c r="A14" s="1">
         <v>0.62280000000000002</v>
       </c>
@@ -5245,8 +5364,11 @@
       <c r="AG14" s="1">
         <v>0.55779999999999996</v>
       </c>
+      <c r="AH14" s="1">
+        <v>0.63980000000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:34">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -5346,8 +5468,11 @@
       <c r="AG15" t="s">
         <v>440</v>
       </c>
+      <c r="AH15" t="s">
+        <v>661</v>
+      </c>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:34">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -5447,8 +5572,11 @@
       <c r="AG16" t="s">
         <v>1129</v>
       </c>
+      <c r="AH16" t="s">
+        <v>1152</v>
+      </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:34">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -5548,8 +5676,11 @@
       <c r="AG17" t="s">
         <v>1130</v>
       </c>
+      <c r="AH17" t="s">
+        <v>1153</v>
+      </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:34">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -5649,8 +5780,11 @@
       <c r="AG18" t="s">
         <v>11</v>
       </c>
+      <c r="AH18" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:34">
       <c r="A19" s="1">
         <v>0.67190000000000005</v>
       </c>
@@ -5750,8 +5884,11 @@
       <c r="AG19" s="1">
         <v>0.63170000000000004</v>
       </c>
+      <c r="AH19" s="1">
+        <v>0.68220000000000003</v>
+      </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:34">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -5851,8 +5988,11 @@
       <c r="AG20" t="s">
         <v>610</v>
       </c>
+      <c r="AH20" t="s">
+        <v>240</v>
+      </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:34">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -5952,8 +6092,11 @@
       <c r="AG21" t="s">
         <v>1131</v>
       </c>
+      <c r="AH21" t="s">
+        <v>1154</v>
+      </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:34">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -6053,8 +6196,11 @@
       <c r="AG22" t="s">
         <v>1132</v>
       </c>
+      <c r="AH22" t="s">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:34">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -6154,8 +6300,11 @@
       <c r="AG23" t="s">
         <v>15</v>
       </c>
+      <c r="AH23" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:34">
       <c r="A24">
         <v>0.83299999999999996</v>
       </c>
@@ -6255,8 +6404,11 @@
       <c r="AG24">
         <v>-0.22</v>
       </c>
+      <c r="AH24">
+        <v>-6.9000000000000006E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:34">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -6356,8 +6508,11 @@
       <c r="AG25" t="s">
         <v>621</v>
       </c>
+      <c r="AH25" t="s">
+        <v>142</v>
+      </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:34">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -6457,8 +6612,11 @@
       <c r="AG26" t="s">
         <v>41</v>
       </c>
+      <c r="AH26" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:34">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -6558,8 +6716,11 @@
       <c r="AG27" t="s">
         <v>41</v>
       </c>
+      <c r="AH27" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:34">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -6659,8 +6820,11 @@
       <c r="AG28" t="s">
         <v>19</v>
       </c>
+      <c r="AH28" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:34">
       <c r="A29">
         <v>82.3</v>
       </c>
@@ -6760,8 +6924,11 @@
       <c r="AG29">
         <v>210</v>
       </c>
+      <c r="AH29">
+        <v>164</v>
+      </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:34">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -6861,8 +7028,11 @@
       <c r="AG30" t="s">
         <v>835</v>
       </c>
+      <c r="AH30" t="s">
+        <v>193</v>
+      </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:34">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -6962,8 +7132,11 @@
       <c r="AG31" t="s">
         <v>1132</v>
       </c>
+      <c r="AH31" t="s">
+        <v>1155</v>
+      </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:34">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -7063,8 +7236,11 @@
       <c r="AG32" t="s">
         <v>323</v>
       </c>
+      <c r="AH32" t="s">
+        <v>1106</v>
+      </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:34">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -7164,8 +7340,11 @@
       <c r="AG33" t="s">
         <v>22</v>
       </c>
+      <c r="AH33" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:34">
       <c r="A34">
         <v>4.1900000000000004</v>
       </c>
@@ -7265,8 +7444,11 @@
       <c r="AG34">
         <v>3.19</v>
       </c>
+      <c r="AH34">
+        <v>3.29</v>
+      </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:34">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -7366,8 +7548,11 @@
       <c r="AG35" t="s">
         <v>455</v>
       </c>
+      <c r="AH35" t="s">
+        <v>281</v>
+      </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:34">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -7467,8 +7652,11 @@
       <c r="AG36" t="s">
         <v>1133</v>
       </c>
+      <c r="AH36" t="s">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:34">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -7568,8 +7756,11 @@
       <c r="AG37" t="s">
         <v>1134</v>
       </c>
+      <c r="AH37" t="s">
+        <v>712</v>
+      </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:34">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -7669,8 +7860,11 @@
       <c r="AG38" t="s">
         <v>26</v>
       </c>
+      <c r="AH38" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:34">
       <c r="A39">
         <v>69.081999999999994</v>
       </c>
@@ -7770,8 +7964,11 @@
       <c r="AG39">
         <v>70.81</v>
       </c>
+      <c r="AH39">
+        <v>70.599999999999994</v>
+      </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:34">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -7871,8 +8068,11 @@
       <c r="AG40" t="s">
         <v>1135</v>
       </c>
+      <c r="AH40" t="s">
+        <v>84</v>
+      </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:34">
       <c r="A41" t="s">
         <v>924</v>
       </c>
@@ -7972,8 +8172,11 @@
       <c r="AG41" t="s">
         <v>1136</v>
       </c>
+      <c r="AH41" t="s">
+        <v>1157</v>
+      </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:34">
       <c r="A42" t="s">
         <v>27</v>
       </c>
@@ -8073,8 +8276,11 @@
       <c r="AG42" t="s">
         <v>1137</v>
       </c>
+      <c r="AH42" t="s">
+        <v>1158</v>
+      </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:34">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -8174,8 +8380,11 @@
       <c r="AG43" t="s">
         <v>28</v>
       </c>
+      <c r="AH43" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:34">
       <c r="A44" s="1">
         <v>0.59260000000000002</v>
       </c>
@@ -8275,8 +8484,11 @@
       <c r="AG44" s="1">
         <v>0.48</v>
       </c>
+      <c r="AH44" s="1">
+        <v>0.48180000000000001</v>
+      </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:34">
       <c r="A45" t="s">
         <v>29</v>
       </c>
@@ -8376,8 +8588,11 @@
       <c r="AG45" t="s">
         <v>618</v>
       </c>
+      <c r="AH45" t="s">
+        <v>252</v>
+      </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:34">
       <c r="A46" t="s">
         <v>30</v>
       </c>
@@ -8477,8 +8692,11 @@
       <c r="AG46" t="s">
         <v>791</v>
       </c>
+      <c r="AH46" t="s">
+        <v>1159</v>
+      </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:34">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -8578,8 +8796,11 @@
       <c r="AG47" t="s">
         <v>96</v>
       </c>
+      <c r="AH47" t="s">
+        <v>1160</v>
+      </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:34">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -8679,8 +8900,11 @@
       <c r="AG48" t="s">
         <v>32</v>
       </c>
+      <c r="AH48" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:34">
       <c r="A49">
         <v>103</v>
       </c>
@@ -8780,8 +9004,11 @@
       <c r="AG49">
         <v>227</v>
       </c>
+      <c r="AH49">
+        <v>170</v>
+      </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:34">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -8881,8 +9108,11 @@
       <c r="AG50" t="s">
         <v>697</v>
       </c>
+      <c r="AH50" t="s">
+        <v>333</v>
+      </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:34">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -8982,8 +9212,11 @@
       <c r="AG51" t="s">
         <v>34</v>
       </c>
+      <c r="AH51" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:34">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -9083,8 +9316,11 @@
       <c r="AG52" t="s">
         <v>35</v>
       </c>
+      <c r="AH52" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:34">
       <c r="A53">
         <v>175</v>
       </c>
@@ -9184,8 +9420,11 @@
       <c r="AG53">
         <v>973</v>
       </c>
+      <c r="AH53">
+        <v>754</v>
+      </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:34">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -9285,8 +9524,11 @@
       <c r="AG54" t="s">
         <v>553</v>
       </c>
+      <c r="AH54" t="s">
+        <v>254</v>
+      </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:34">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -9386,8 +9628,11 @@
       <c r="AG55" t="s">
         <v>36</v>
       </c>
+      <c r="AH55" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:34">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -9487,8 +9732,11 @@
       <c r="AG56" t="s">
         <v>98</v>
       </c>
+      <c r="AH56" t="s">
+        <v>98</v>
+      </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:34">
       <c r="A57" s="2">
         <v>2380</v>
       </c>
@@ -9588,8 +9836,11 @@
       <c r="AG57">
         <v>724</v>
       </c>
+      <c r="AH57">
+        <v>858</v>
+      </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:34">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -9689,8 +9940,11 @@
       <c r="AG58" t="s">
         <v>131</v>
       </c>
+      <c r="AH58" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:34">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -9790,8 +10044,11 @@
       <c r="AG59" t="s">
         <v>1138</v>
       </c>
+      <c r="AH59" t="s">
+        <v>1161</v>
+      </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:34">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -9891,8 +10148,11 @@
       <c r="AG60" t="s">
         <v>41</v>
       </c>
+      <c r="AH60" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:34">
       <c r="A61" t="s">
         <v>40</v>
       </c>
@@ -9992,8 +10252,11 @@
       <c r="AG61" t="s">
         <v>99</v>
       </c>
+      <c r="AH61" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:34">
       <c r="A62" s="3">
         <v>5909742</v>
       </c>
@@ -10093,8 +10356,11 @@
       <c r="AG62" s="2">
         <v>1102</v>
       </c>
+      <c r="AH62" s="2">
+        <v>1206</v>
+      </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:34">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -10194,8 +10460,11 @@
       <c r="AG63" t="s">
         <v>181</v>
       </c>
+      <c r="AH63" t="s">
+        <v>296</v>
+      </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:34">
       <c r="A64" t="s">
         <v>41</v>
       </c>
@@ -10295,8 +10564,11 @@
       <c r="AG64" t="s">
         <v>1139</v>
       </c>
+      <c r="AH64" t="s">
+        <v>1162</v>
+      </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:34">
       <c r="A65" t="s">
         <v>42</v>
       </c>
@@ -10396,8 +10668,11 @@
       <c r="AG65" t="s">
         <v>1140</v>
       </c>
+      <c r="AH65" t="s">
+        <v>1163</v>
+      </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:34">
       <c r="A66" t="s">
         <v>43</v>
       </c>
@@ -10497,8 +10772,11 @@
       <c r="AG66" t="s">
         <v>40</v>
       </c>
+      <c r="AH66" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:34">
       <c r="A67" s="1">
         <v>0.24479999999999999</v>
       </c>
@@ -10598,8 +10876,11 @@
       <c r="AG67" s="3">
         <v>1483948</v>
       </c>
+      <c r="AH67" s="3">
+        <v>1859040</v>
+      </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:34">
       <c r="A68" t="s">
         <v>44</v>
       </c>
@@ -10699,8 +10980,11 @@
       <c r="AG68" t="s">
         <v>374</v>
       </c>
+      <c r="AH68" t="s">
+        <v>826</v>
+      </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:34">
       <c r="A69" t="s">
         <v>45</v>
       </c>
@@ -10800,8 +11084,11 @@
       <c r="AG69" t="s">
         <v>41</v>
       </c>
+      <c r="AH69" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:34">
       <c r="A70" t="s">
         <v>46</v>
       </c>
@@ -10901,8 +11188,11 @@
       <c r="AG70" t="s">
         <v>41</v>
       </c>
+      <c r="AH70" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:34">
       <c r="A71" t="s">
         <v>47</v>
       </c>
@@ -11002,8 +11292,11 @@
       <c r="AG71" t="s">
         <v>43</v>
       </c>
+      <c r="AH71" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:34">
       <c r="A72" s="1">
         <v>0.46200000000000002</v>
       </c>
@@ -11103,8 +11396,11 @@
       <c r="AG72" s="1">
         <v>0.1817</v>
       </c>
+      <c r="AH72" s="1">
+        <v>0.189</v>
+      </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:34">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -11204,8 +11500,11 @@
       <c r="AG73" t="s">
         <v>440</v>
       </c>
+      <c r="AH73" t="s">
+        <v>287</v>
+      </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:34">
       <c r="A74" t="s">
         <v>49</v>
       </c>
@@ -11305,8 +11604,11 @@
       <c r="AG74" t="s">
         <v>1141</v>
       </c>
+      <c r="AH74" t="s">
+        <v>429</v>
+      </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:34">
       <c r="A75" t="s">
         <v>50</v>
       </c>
@@ -11406,8 +11708,11 @@
       <c r="AG75" t="s">
         <v>1142</v>
       </c>
+      <c r="AH75" t="s">
+        <v>1164</v>
+      </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:34">
       <c r="A76" t="s">
         <v>51</v>
       </c>
@@ -11507,8 +11812,11 @@
       <c r="AG76" t="s">
         <v>47</v>
       </c>
+      <c r="AH76" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:34">
       <c r="A77" t="s">
         <v>52</v>
       </c>
@@ -11608,8 +11916,11 @@
       <c r="AG77" s="1">
         <v>0.40699999999999997</v>
       </c>
+      <c r="AH77" s="1">
+        <v>0.57099999999999995</v>
+      </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:34">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -11709,8 +12020,11 @@
       <c r="AG78" t="s">
         <v>287</v>
       </c>
+      <c r="AH78" t="s">
+        <v>436</v>
+      </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:34">
       <c r="A79" t="s">
         <v>3</v>
       </c>
@@ -11810,8 +12124,11 @@
       <c r="AG79" t="s">
         <v>41</v>
       </c>
+      <c r="AH79" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:34">
       <c r="A80" t="s">
         <v>53</v>
       </c>
@@ -11911,8 +12228,11 @@
       <c r="AG80" t="s">
         <v>41</v>
       </c>
+      <c r="AH80" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:34">
       <c r="A81" s="1">
         <v>0.1484</v>
       </c>
@@ -12012,8 +12332,11 @@
       <c r="AG81" t="s">
         <v>51</v>
       </c>
+      <c r="AH81" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:34">
       <c r="A82" t="s">
         <v>54</v>
       </c>
@@ -12113,8 +12436,11 @@
       <c r="AG82" t="s">
         <v>52</v>
       </c>
+      <c r="AH82" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:34">
       <c r="A83" t="s">
         <v>55</v>
       </c>
@@ -12214,8 +12540,11 @@
       <c r="AG83" t="s">
         <v>2</v>
       </c>
+      <c r="AH83" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:34">
       <c r="A84" t="s">
         <v>56</v>
       </c>
@@ -12315,8 +12644,11 @@
       <c r="AG84" t="s">
         <v>3</v>
       </c>
+      <c r="AH84" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:34">
       <c r="A85" t="s">
         <v>57</v>
       </c>
@@ -12416,8 +12748,11 @@
       <c r="AG85" t="s">
         <v>53</v>
       </c>
+      <c r="AH85" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:34">
       <c r="A86" s="1">
         <v>0.17560000000000001</v>
       </c>
@@ -12517,8 +12852,11 @@
       <c r="AG86" s="1">
         <v>0.12720000000000001</v>
       </c>
+      <c r="AH86" s="1">
+        <v>0.11210000000000001</v>
+      </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:34">
       <c r="A87" t="s">
         <v>58</v>
       </c>
@@ -12618,8 +12956,11 @@
       <c r="AG87" t="s">
         <v>313</v>
       </c>
+      <c r="AH87" t="s">
+        <v>675</v>
+      </c>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:34">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -12719,8 +13060,11 @@
       <c r="AG88" t="s">
         <v>266</v>
       </c>
+      <c r="AH88" t="s">
+        <v>266</v>
+      </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:34">
       <c r="A89" t="s">
         <v>60</v>
       </c>
@@ -12820,8 +13164,11 @@
       <c r="AG89" t="s">
         <v>267</v>
       </c>
+      <c r="AH89" t="s">
+        <v>1165</v>
+      </c>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:34">
       <c r="A90" t="s">
         <v>61</v>
       </c>
@@ -12921,8 +13268,11 @@
       <c r="AG90" t="s">
         <v>57</v>
       </c>
+      <c r="AH90" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:34">
       <c r="A91" s="1">
         <v>0.5625</v>
       </c>
@@ -13022,8 +13372,11 @@
       <c r="AG91" s="1">
         <v>0.1454</v>
       </c>
+      <c r="AH91" s="1">
+        <v>0.15390000000000001</v>
+      </c>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:34">
       <c r="A92" t="s">
         <v>62</v>
       </c>
@@ -13123,8 +13476,11 @@
       <c r="AG92" t="s">
         <v>522</v>
       </c>
+      <c r="AH92" t="s">
+        <v>397</v>
+      </c>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:34">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -13224,8 +13580,11 @@
       <c r="AG93" t="s">
         <v>614</v>
       </c>
+      <c r="AH93" t="s">
+        <v>1166</v>
+      </c>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:34">
       <c r="A94" t="s">
         <v>64</v>
       </c>
@@ -13325,8 +13684,11 @@
       <c r="AG94" t="s">
         <v>1143</v>
       </c>
+      <c r="AH94" t="s">
+        <v>1167</v>
+      </c>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:34">
       <c r="A95" t="s">
         <v>65</v>
       </c>
@@ -13426,8 +13788,11 @@
       <c r="AG95" t="s">
         <v>61</v>
       </c>
+      <c r="AH95" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:34">
       <c r="A96" s="1">
         <v>0.3523</v>
       </c>
@@ -13527,8 +13892,11 @@
       <c r="AG96" s="1">
         <v>0.4093</v>
       </c>
+      <c r="AH96" s="1">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:34">
       <c r="A97" t="s">
         <v>44</v>
       </c>
@@ -13628,8 +13996,11 @@
       <c r="AG97" t="s">
         <v>618</v>
       </c>
+      <c r="AH97" t="s">
+        <v>336</v>
+      </c>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:34">
       <c r="A98" t="s">
         <v>66</v>
       </c>
@@ -13729,8 +14100,11 @@
       <c r="AG98" t="s">
         <v>822</v>
       </c>
+      <c r="AH98" t="s">
+        <v>458</v>
+      </c>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:34">
       <c r="A99" t="s">
         <v>67</v>
       </c>
@@ -13830,8 +14204,11 @@
       <c r="AG99" t="s">
         <v>1144</v>
       </c>
+      <c r="AH99" t="s">
+        <v>1168</v>
+      </c>
     </row>
-    <row r="100" spans="1:33">
+    <row r="100" spans="1:34">
       <c r="A100" t="s">
         <v>51</v>
       </c>
@@ -13931,8 +14308,11 @@
       <c r="AG100" t="s">
         <v>65</v>
       </c>
+      <c r="AH100" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:34">
       <c r="A101" t="s">
         <v>68</v>
       </c>
@@ -14032,8 +14412,11 @@
       <c r="AG101" s="1">
         <v>0.27010000000000001</v>
       </c>
+      <c r="AH101" s="1">
+        <v>0.26769999999999999</v>
+      </c>
     </row>
-    <row r="102" spans="1:33">
+    <row r="102" spans="1:34">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -14133,8 +14516,11 @@
       <c r="AG102" t="s">
         <v>697</v>
       </c>
+      <c r="AH102" t="s">
+        <v>595</v>
+      </c>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:34">
       <c r="A103" t="s">
         <v>3</v>
       </c>
@@ -14234,8 +14620,11 @@
       <c r="AG103" t="s">
         <v>1145</v>
       </c>
+      <c r="AH103" t="s">
+        <v>1169</v>
+      </c>
     </row>
-    <row r="104" spans="1:33">
+    <row r="104" spans="1:34">
       <c r="A104" t="s">
         <v>69</v>
       </c>
@@ -14335,8 +14724,11 @@
       <c r="AG104" t="s">
         <v>1131</v>
       </c>
+      <c r="AH104" t="s">
+        <v>1170</v>
+      </c>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:34">
       <c r="A105">
         <v>70.28</v>
       </c>
@@ -14433,8 +14825,11 @@
       <c r="AG105" t="s">
         <v>51</v>
       </c>
+      <c r="AH105" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:34">
       <c r="A106" t="s">
         <v>70</v>
       </c>
@@ -14531,8 +14926,11 @@
       <c r="AG106" t="s">
         <v>68</v>
       </c>
+      <c r="AH106" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:34">
       <c r="A107" t="s">
         <v>924</v>
       </c>
@@ -14629,8 +15027,11 @@
       <c r="AG107" t="s">
         <v>2</v>
       </c>
+      <c r="AH107" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:34">
       <c r="A108" t="s">
         <v>25</v>
       </c>
@@ -14727,8 +15128,11 @@
       <c r="AG108" t="s">
         <v>3</v>
       </c>
+      <c r="AH108" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:34">
       <c r="A109" t="s">
         <v>71</v>
       </c>
@@ -14825,8 +15229,11 @@
       <c r="AG109" t="s">
         <v>69</v>
       </c>
+      <c r="AH109" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:34">
       <c r="A110">
         <v>69.25</v>
       </c>
@@ -14923,8 +15330,11 @@
       <c r="AG110">
         <v>71.290000000000006</v>
       </c>
+      <c r="AH110">
+        <v>70.790000000000006</v>
+      </c>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:34">
       <c r="A111" t="s">
         <v>20</v>
       </c>
@@ -15021,8 +15431,11 @@
       <c r="AG111" t="s">
         <v>443</v>
       </c>
+      <c r="AH111" t="s">
+        <v>411</v>
+      </c>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:34">
       <c r="A112" t="s">
         <v>1020</v>
       </c>
@@ -15119,8 +15532,11 @@
       <c r="AG112" t="s">
         <v>1136</v>
       </c>
+      <c r="AH112" t="s">
+        <v>1157</v>
+      </c>
     </row>
-    <row r="113" spans="1:33">
+    <row r="113" spans="1:34">
       <c r="A113" t="s">
         <v>72</v>
       </c>
@@ -15217,8 +15633,11 @@
       <c r="AG113" t="s">
         <v>1134</v>
       </c>
+      <c r="AH113" t="s">
+        <v>712</v>
+      </c>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:34">
       <c r="A114" t="s">
         <v>73</v>
       </c>
@@ -15315,8 +15734,11 @@
       <c r="AG114" t="s">
         <v>71</v>
       </c>
+      <c r="AH114" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:34">
       <c r="A115">
         <v>71</v>
       </c>
@@ -15410,8 +15832,11 @@
       <c r="AG115">
         <v>71.599999999999994</v>
       </c>
+      <c r="AH115">
+        <v>70.69</v>
+      </c>
     </row>
-    <row r="116" spans="1:33">
+    <row r="116" spans="1:34">
       <c r="A116" t="s">
         <v>74</v>
       </c>
@@ -15505,8 +15930,11 @@
       <c r="AG116" t="s">
         <v>408</v>
       </c>
+      <c r="AH116" t="s">
+        <v>262</v>
+      </c>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:34">
       <c r="A117" t="s">
         <v>75</v>
       </c>
@@ -15600,8 +16028,11 @@
       <c r="AG117" t="s">
         <v>1146</v>
       </c>
+      <c r="AH117" t="s">
+        <v>1171</v>
+      </c>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:34">
       <c r="A118" t="s">
         <v>76</v>
       </c>
@@ -15695,8 +16126,11 @@
       <c r="AG118" t="s">
         <v>437</v>
       </c>
+      <c r="AH118" t="s">
+        <v>1172</v>
+      </c>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:34">
       <c r="A119" t="s">
         <v>77</v>
       </c>
@@ -15790,8 +16224,11 @@
       <c r="AG119" t="s">
         <v>73</v>
       </c>
+      <c r="AH119" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:34">
       <c r="A120">
         <v>71.63</v>
       </c>
@@ -15882,8 +16319,11 @@
       <c r="AG120">
         <v>69.83</v>
       </c>
+      <c r="AH120">
+        <v>70.72</v>
+      </c>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:34">
       <c r="A121" t="s">
         <v>78</v>
       </c>
@@ -15974,8 +16414,11 @@
       <c r="AG121" t="s">
         <v>12</v>
       </c>
+      <c r="AH121" t="s">
+        <v>825</v>
+      </c>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:34">
       <c r="A122" t="s">
         <v>79</v>
       </c>
@@ -16066,8 +16509,11 @@
       <c r="AG122" t="s">
         <v>1147</v>
       </c>
+      <c r="AH122" t="s">
+        <v>1173</v>
+      </c>
     </row>
-    <row r="123" spans="1:33">
+    <row r="123" spans="1:34">
       <c r="A123" t="s">
         <v>76</v>
       </c>
@@ -16158,8 +16604,11 @@
       <c r="AG123" t="s">
         <v>495</v>
       </c>
+      <c r="AH123" t="s">
+        <v>463</v>
+      </c>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:34">
       <c r="B124" t="s">
         <v>77</v>
       </c>
@@ -16217,8 +16666,11 @@
       <c r="AG124" t="s">
         <v>77</v>
       </c>
+      <c r="AH124" t="s">
+        <v>77</v>
+      </c>
     </row>
-    <row r="125" spans="1:33">
+    <row r="125" spans="1:34">
       <c r="B125">
         <v>70.400000000000006</v>
       </c>
@@ -16273,8 +16725,11 @@
       <c r="AG125">
         <v>71.33</v>
       </c>
+      <c r="AH125">
+        <v>71.06</v>
+      </c>
     </row>
-    <row r="126" spans="1:33">
+    <row r="126" spans="1:34">
       <c r="B126" t="s">
         <v>114</v>
       </c>
@@ -16329,8 +16784,11 @@
       <c r="AG126" t="s">
         <v>540</v>
       </c>
+      <c r="AH126" t="s">
+        <v>498</v>
+      </c>
     </row>
-    <row r="127" spans="1:33">
+    <row r="127" spans="1:34">
       <c r="B127" t="s">
         <v>1060</v>
       </c>
@@ -16385,8 +16843,11 @@
       <c r="AG127" t="s">
         <v>1148</v>
       </c>
+      <c r="AH127" t="s">
+        <v>1174</v>
+      </c>
     </row>
-    <row r="128" spans="1:33">
+    <row r="128" spans="1:34">
       <c r="B128" t="s">
         <v>115</v>
       </c>
@@ -16440,6 +16901,9 @@
       </c>
       <c r="AG128" t="s">
         <v>495</v>
+      </c>
+      <c r="AH128" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>